<commit_message>
AirplanePlus, Interkosmos, and Kraken Science Support
Added AirplanePlus, Interkosmos, and Kraken Science Support; Lowered data scale of early science; Added 20 EC to probes to help balance lack of start battery; Lowered cost of radio experiments in LTech; Moved Circular Intake earlier; Moved the L-02 Beehive LaunchPad (Luciole) support for modular launch pads.
</commit_message>
<xml_diff>
--- a/Source/JetEngineUpgrade.xlsx
+++ b/Source/JetEngineUpgrade.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\3D\KSP\kiwiTechTree\Source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C66F102-DE8A-4D5B-A75C-48482D0AF557}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48C294BB-6676-4DED-B813-C1551FEFDC79}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14745" yWindow="0" windowWidth="14655" windowHeight="9975" xr2:uid="{29C0BFBB-DC5B-4724-B31D-EBBB33A08879}"/>
+    <workbookView xWindow="-9915" yWindow="0" windowWidth="9630" windowHeight="15600" xr2:uid="{29C0BFBB-DC5B-4724-B31D-EBBB33A08879}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -411,7 +411,7 @@
   <dimension ref="D1:L10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -443,18 +443,18 @@
         <v>1</v>
       </c>
       <c r="E3">
-        <v>210</v>
+        <v>65</v>
       </c>
       <c r="F3">
         <f>E3*1.2</f>
-        <v>252</v>
+        <v>78</v>
       </c>
       <c r="G3">
-        <v>330</v>
+        <v>140</v>
       </c>
       <c r="H3">
         <f>G3*1.2</f>
-        <v>396</v>
+        <v>168</v>
       </c>
     </row>
     <row r="4" spans="4:12" x14ac:dyDescent="0.35">
@@ -462,18 +462,18 @@
         <v>2</v>
       </c>
       <c r="E4">
-        <v>148.018</v>
+        <v>65.001999999999995</v>
       </c>
       <c r="F4">
         <f>F3*E5</f>
-        <v>177.6216</v>
+        <v>78.00239999999998</v>
       </c>
       <c r="G4">
-        <v>330.42</v>
+        <v>236.37200000000001</v>
       </c>
       <c r="H4">
         <f>H3*G5</f>
-        <v>396.50400000000002</v>
+        <v>283.64640000000003</v>
       </c>
     </row>
     <row r="5" spans="4:12" x14ac:dyDescent="0.35">
@@ -482,7 +482,7 @@
       </c>
       <c r="E5">
         <f>E4/E3</f>
-        <v>0.70484761904761906</v>
+        <v>1.0000307692307691</v>
       </c>
       <c r="F5">
         <f>3600*0.9</f>
@@ -490,7 +490,7 @@
       </c>
       <c r="G5">
         <f>G4/G3</f>
-        <v>1.0012727272727273</v>
+        <v>1.6883714285714286</v>
       </c>
       <c r="H5">
         <f>3600*0.9</f>
@@ -502,18 +502,18 @@
         <v>6</v>
       </c>
       <c r="E7">
-        <v>29000</v>
+        <v>3000</v>
       </c>
       <c r="F7">
         <f>E7*1.5</f>
-        <v>43500</v>
+        <v>4500</v>
       </c>
       <c r="G7">
-        <v>12400</v>
+        <v>4400</v>
       </c>
       <c r="H7">
         <f>G7*1.5</f>
-        <v>18600</v>
+        <v>6600</v>
       </c>
     </row>
     <row r="10" spans="4:12" x14ac:dyDescent="0.35">

</xml_diff>